<commit_message>
fixed #7, replaced USB connector part.# on BOM
</commit_message>
<xml_diff>
--- a/_Output/BOM/BOM-BLEUART-USB-Dongle.xlsx
+++ b/_Output/BOM/BOM-BLEUART-USB-Dongle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angrypig\Dev\NEO3DS-PCB\_Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angrypig\Dev\NEO3DS-PCB\_Output\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6AAE90-8966-4FC6-9643-1A41D7CA206F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8839E22E-C0F7-4B37-8F74-291F5247ABC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,9 +239,6 @@
     <t>C85364</t>
   </si>
   <si>
-    <t>C98125</t>
-  </si>
-  <si>
     <t>C17168</t>
   </si>
   <si>
@@ -287,12 +284,6 @@
     <t>NCD0603O1</t>
   </si>
   <si>
-    <t>Korean Hroparts Elec</t>
-  </si>
-  <si>
-    <t>U-G-O4DD-W-1</t>
-  </si>
-  <si>
     <t>USB2.0 Type-A Male Connector</t>
   </si>
   <si>
@@ -360,6 +351,15 @@
   </si>
   <si>
     <t>C25918</t>
+  </si>
+  <si>
+    <t>Jing Extension of the Electronic Co.</t>
+  </si>
+  <si>
+    <t>917-181A102ED60200</t>
+  </si>
+  <si>
+    <t>C9739</t>
   </si>
 </sst>
 </file>
@@ -759,7 +759,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Header!$B$2:$R$4" spid="_x0000_s2312"/>
+                  <a14:cameraTool cellRange="Header!$B$2:$R$4" spid="_x0000_s2317"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1068,7 +1068,7 @@
   <dimension ref="A6:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,10 +1267,10 @@
         <v>51</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
@@ -1291,16 +1291,16 @@
         <v>18</v>
       </c>
       <c r="F15" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>83</v>
-      </c>
       <c r="H15" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -1317,16 +1317,16 @@
         <v>18</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1342,17 +1342,17 @@
       <c r="E17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>85</v>
+      <c r="F17" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>23</v>
@@ -1392,7 +1392,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1455,16 +1455,16 @@
         <v>45</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>44</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1478,19 +1478,19 @@
         <v>47</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F23" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>96</v>
-      </c>
       <c r="I23" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -1507,14 +1507,14 @@
         <v>42</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -1531,16 +1531,16 @@
         <v>56</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -1557,16 +1557,16 @@
         <v>55</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="34" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E2" s="35"/>
       <c r="F2" s="35"/>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>

</xml_diff>